<commit_message>
fixed crew number logic(working)
</commit_message>
<xml_diff>
--- a/roaster/input/input1.xlsx
+++ b/roaster/input/input1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26100" windowHeight="17160"/>
+    <workbookView windowWidth="32040" windowHeight="15320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2291,7 +2291,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" customHeight="1"/>

</xml_diff>